<commit_message>
Update expected outputs using 10-13-22 PEARS schema
</commit_message>
<xml_diff>
--- a/tests/expected_outputs/CPHP Staff PEARS Entries 2022-09.xlsx
+++ b/tests/expected_outputs/CPHP Staff PEARS Entries 2022-09.xlsx
@@ -154,148 +154,148 @@
     <t>Success Stories Collaborated Created YTD</t>
   </si>
   <si>
-    <t>Anita Theresa. Cook</t>
-  </si>
-  <si>
-    <t>Chad Craig</t>
-  </si>
-  <si>
-    <t>Christopher Berry</t>
-  </si>
-  <si>
-    <t>Daisy Jackson</t>
-  </si>
-  <si>
-    <t>DarCorey Noble</t>
-  </si>
-  <si>
-    <t>Dominique I. Harper</t>
-  </si>
-  <si>
-    <t>Gabriel D.  Schneider</t>
-  </si>
-  <si>
-    <t>Jennifer Jones</t>
-  </si>
-  <si>
-    <t>Jesse Munoz</t>
-  </si>
-  <si>
-    <t>Karinalas R. Schneider</t>
-  </si>
-  <si>
-    <t>Lauren A. Huffman</t>
-  </si>
-  <si>
-    <t>Micheller Robinson</t>
-  </si>
-  <si>
-    <t>Neil Mendoza</t>
-  </si>
-  <si>
-    <t>Scottan Ewing</t>
-  </si>
-  <si>
-    <t>Scottanette Jones</t>
-  </si>
-  <si>
-    <t>Stephen Michael</t>
-  </si>
-  <si>
-    <t>Thomas Martin</t>
-  </si>
-  <si>
-    <t>Tiffany Theresa. Martinez</t>
-  </si>
-  <si>
-    <t>Timothy  Smith</t>
-  </si>
-  <si>
-    <t>Timothy Kimberly Brown</t>
-  </si>
-  <si>
-    <t>Tina Pruitt</t>
-  </si>
-  <si>
-    <t>Toni Williams</t>
-  </si>
-  <si>
-    <t>Yvonne Williams</t>
-  </si>
-  <si>
-    <t>Zachary Hodge</t>
-  </si>
-  <si>
-    <t>Anita.Cook@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Chad.Craig@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Christopher.Berry@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Daisy.Ramirez@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Mary.Noble@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Dominique.Harper@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Gabriel.Glenn@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Jennifer.Jones@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Jesse.Munoz@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Jordan.Williams@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Lauren.Huffman@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Michelle.Robinson@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Neil.Mendoza@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Darius.Ewing@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Abigail.Hawkins.DVM@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Stephen.Michael@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Thomas.Martin@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Tiffany.Martinez@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Timothy.Fritz@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Timothy.Brown@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Melissa.Pruitt@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Theresa.Williams@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Yvonne.Williams@fake_domain.com</t>
-  </si>
-  <si>
-    <t>Zachary.Hodge@fake_domain.com</t>
+    <t>Anthony Mclaughlin</t>
+  </si>
+  <si>
+    <t>Brandon Cox</t>
+  </si>
+  <si>
+    <t>Bryan Chapman</t>
+  </si>
+  <si>
+    <t>Caitlin Brown</t>
+  </si>
+  <si>
+    <t>Chelsear Harper</t>
+  </si>
+  <si>
+    <t>Christopher Foster</t>
+  </si>
+  <si>
+    <t>Daniel Marissa Poole</t>
+  </si>
+  <si>
+    <t>DarJason Mccullough</t>
+  </si>
+  <si>
+    <t>David A. Phillips</t>
+  </si>
+  <si>
+    <t>Derek Johnson</t>
+  </si>
+  <si>
+    <t>Garyan Gonzales</t>
+  </si>
+  <si>
+    <t>Garyanette Hill</t>
+  </si>
+  <si>
+    <t>Jackson Glenda. Baker</t>
+  </si>
+  <si>
+    <t>James I. Grant</t>
+  </si>
+  <si>
+    <t>Jamie  Ward</t>
+  </si>
+  <si>
+    <t>Jennifer Carr</t>
+  </si>
+  <si>
+    <t>John Rogers</t>
+  </si>
+  <si>
+    <t>Kari Glenda. Griffith</t>
+  </si>
+  <si>
+    <t>Kayleelas R. Clay</t>
+  </si>
+  <si>
+    <t>Kyle Thompson</t>
+  </si>
+  <si>
+    <t>Mary Williams</t>
+  </si>
+  <si>
+    <t>Matthew Oconnor</t>
+  </si>
+  <si>
+    <t>Reginald D.  Clay</t>
+  </si>
+  <si>
+    <t>Wendy Young</t>
+  </si>
+  <si>
+    <t>Anthony.Mclaughlin@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Brandon.Cox@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Bryan.Chapman@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Caitlin.Brown@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Chelsea.Harper@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Christopher.Foster@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Daniel.Poole@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Joann.Mccullough@fake_domain.com</t>
+  </si>
+  <si>
+    <t>David.Phillips@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Daniel.Johnson@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Angela.Gonzales@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Charles.Smith@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Jackson.Baker@fake_domain.com</t>
+  </si>
+  <si>
+    <t>James.Grant@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Jamie.Butler@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Jennifer.Carr@fake_domain.com</t>
+  </si>
+  <si>
+    <t>John.Rogers@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Kari.Griffith@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Wayne.Johnston@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Kyle.Thompson@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Mary.Stark@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Matthew.Oconnor@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Reginald.Barker@fake_domain.com</t>
+  </si>
+  <si>
+    <t>Monique.Young@fake_domain.com</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -861,7 +861,7 @@
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
@@ -873,37 +873,37 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -921,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -945,37 +945,37 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="AH2">
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AK2">
         <v>0</v>
       </c>
       <c r="AL2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AN2">
         <v>0</v>
@@ -1144,58 +1144,58 @@
         <v>71</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>7</v>
       </c>
       <c r="H4">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="I4">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1210,46 +1210,46 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE4">
         <v>1</v>
       </c>
       <c r="AF4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AG4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AH4">
         <v>0</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="AM4">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="AN4">
         <v>0</v>
@@ -1261,18 +1261,18 @@
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AS4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:45">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
@@ -1290,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1311,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1326,13 +1326,13 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1347,10 +1347,10 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB5">
         <v>0</v>
@@ -1362,13 +1362,13 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AH5">
         <v>0</v>
@@ -1380,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="AK5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AN5">
         <v>0</v>
@@ -1398,13 +1398,13 @@
         <v>0</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -1418,40 +1418,40 @@
         <v>73</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H6">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O6">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -1478,52 +1478,52 @@
         <v>0</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD6">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF6">
         <v>4</v>
       </c>
       <c r="AG6">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="AH6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL6">
         <v>3</v>
       </c>
       <c r="AM6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AN6">
         <v>0</v>
@@ -1555,130 +1555,130 @@
         <v>74</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F7">
+        <v>58</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>95</v>
+      </c>
+      <c r="I7">
+        <v>96</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+      <c r="O7">
+        <v>13</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>27</v>
+      </c>
+      <c r="U7">
+        <v>27</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>3</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>4</v>
+      </c>
+      <c r="AA7">
+        <v>4</v>
+      </c>
+      <c r="AB7">
+        <v>6</v>
+      </c>
+      <c r="AC7">
         <v>25</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>54</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>16</v>
-      </c>
-      <c r="L7">
-        <v>20</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>17</v>
-      </c>
-      <c r="O7">
-        <v>35</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
       <c r="AD7">
+        <v>25</v>
+      </c>
+      <c r="AE7">
+        <v>6</v>
+      </c>
+      <c r="AF7">
+        <v>25</v>
+      </c>
+      <c r="AG7">
+        <v>25</v>
+      </c>
+      <c r="AH7">
+        <v>4</v>
+      </c>
+      <c r="AI7">
+        <v>12</v>
+      </c>
+      <c r="AJ7">
+        <v>12</v>
+      </c>
+      <c r="AK7">
+        <v>5</v>
+      </c>
+      <c r="AL7">
+        <v>22</v>
+      </c>
+      <c r="AM7">
+        <v>22</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
         <v>3</v>
       </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <v>17</v>
-      </c>
-      <c r="AH7">
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-      <c r="AJ7">
-        <v>2</v>
-      </c>
-      <c r="AK7">
-        <v>0</v>
-      </c>
-      <c r="AL7">
-        <v>0</v>
-      </c>
-      <c r="AM7">
-        <v>2</v>
-      </c>
-      <c r="AN7">
-        <v>0</v>
-      </c>
-      <c r="AO7">
-        <v>0</v>
-      </c>
       <c r="AP7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -1692,22 +1692,22 @@
         <v>75</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1746,59 +1746,59 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <v>2</v>
       </c>
       <c r="Y8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>20</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>21</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>2</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
         <v>5</v>
       </c>
-      <c r="AC8">
-        <v>5</v>
-      </c>
-      <c r="AD8">
-        <v>5</v>
-      </c>
-      <c r="AE8">
-        <v>5</v>
-      </c>
-      <c r="AF8">
-        <v>5</v>
-      </c>
-      <c r="AG8">
-        <v>5</v>
-      </c>
-      <c r="AH8">
-        <v>1</v>
-      </c>
-      <c r="AI8">
-        <v>1</v>
-      </c>
-      <c r="AJ8">
-        <v>1</v>
-      </c>
-      <c r="AK8">
-        <v>1</v>
-      </c>
-      <c r="AL8">
-        <v>1</v>
-      </c>
-      <c r="AM8">
-        <v>1</v>
-      </c>
       <c r="AN8">
         <v>0</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="AP8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ8">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="AS8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -1829,112 +1829,112 @@
         <v>76</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I9">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="J9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N9">
+        <v>13</v>
+      </c>
+      <c r="O9">
+        <v>74</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>22</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>4</v>
+      </c>
+      <c r="AG9">
+        <v>30</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>3</v>
+      </c>
+      <c r="AM9">
         <v>9</v>
-      </c>
-      <c r="O9">
-        <v>9</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-      <c r="AC9">
-        <v>10</v>
-      </c>
-      <c r="AD9">
-        <v>10</v>
-      </c>
-      <c r="AE9">
-        <v>1</v>
-      </c>
-      <c r="AF9">
-        <v>10</v>
-      </c>
-      <c r="AG9">
-        <v>10</v>
-      </c>
-      <c r="AH9">
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <v>8</v>
-      </c>
-      <c r="AJ9">
-        <v>8</v>
-      </c>
-      <c r="AK9">
-        <v>0</v>
-      </c>
-      <c r="AL9">
-        <v>8</v>
-      </c>
-      <c r="AM9">
-        <v>8</v>
       </c>
       <c r="AN9">
         <v>0</v>
@@ -1966,40 +1966,40 @@
         <v>77</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>47</v>
+      </c>
+      <c r="J10">
+        <v>7</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>13</v>
+      </c>
+      <c r="M10">
+        <v>7</v>
+      </c>
+      <c r="N10">
         <v>8</v>
       </c>
-      <c r="F10">
-        <v>36</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>16</v>
-      </c>
-      <c r="I10">
-        <v>61</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>8</v>
-      </c>
-      <c r="L10">
-        <v>29</v>
-      </c>
-      <c r="M10">
-        <v>8</v>
-      </c>
-      <c r="N10">
-        <v>16</v>
-      </c>
       <c r="O10">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -2008,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="AF10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <v>16</v>
@@ -2059,19 +2059,19 @@
         <v>0</v>
       </c>
       <c r="AI10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK10">
         <v>0</v>
       </c>
       <c r="AL10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AN10">
         <v>0</v>
@@ -2103,67 +2103,67 @@
         <v>78</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F11">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="I11">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
         <v>8</v>
       </c>
-      <c r="L11">
-        <v>10</v>
-      </c>
-      <c r="M11">
-        <v>2</v>
-      </c>
-      <c r="N11">
+      <c r="R11">
+        <v>8</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
         <v>16</v>
       </c>
-      <c r="O11">
-        <v>20</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>2</v>
-      </c>
       <c r="U11">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="V11">
         <v>0</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11">
         <v>0</v>
@@ -2178,55 +2178,55 @@
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE11">
         <v>0</v>
       </c>
       <c r="AF11">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="AG11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="AH11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AK11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL11">
+        <v>16</v>
+      </c>
+      <c r="AM11">
+        <v>16</v>
+      </c>
+      <c r="AN11">
+        <v>1</v>
+      </c>
+      <c r="AO11">
+        <v>2</v>
+      </c>
+      <c r="AP11">
+        <v>2</v>
+      </c>
+      <c r="AQ11">
+        <v>2</v>
+      </c>
+      <c r="AR11">
         <v>6</v>
       </c>
-      <c r="AM11">
+      <c r="AS11">
         <v>6</v>
-      </c>
-      <c r="AN11">
-        <v>0</v>
-      </c>
-      <c r="AO11">
-        <v>0</v>
-      </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-      <c r="AR11">
-        <v>0</v>
-      </c>
-      <c r="AS11">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -2240,40 +2240,40 @@
         <v>79</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="O12">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="AD12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE12">
         <v>0</v>
@@ -2333,19 +2333,19 @@
         <v>0</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK12">
         <v>0</v>
       </c>
       <c r="AL12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AN12">
         <v>0</v>
@@ -2377,22 +2377,22 @@
         <v>80</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2401,16 +2401,16 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2437,52 +2437,52 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD13">
         <v>3</v>
       </c>
       <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>18</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
         <v>3</v>
       </c>
-      <c r="AF13">
-        <v>4</v>
-      </c>
-      <c r="AG13">
-        <v>8</v>
-      </c>
-      <c r="AH13">
-        <v>2</v>
-      </c>
-      <c r="AI13">
-        <v>2</v>
-      </c>
-      <c r="AJ13">
-        <v>2</v>
-      </c>
       <c r="AK13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
         <v>3</v>
-      </c>
-      <c r="AM13">
-        <v>6</v>
       </c>
       <c r="AN13">
         <v>0</v>
@@ -2514,130 +2514,130 @@
         <v>81</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <v>24</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>10</v>
       </c>
-      <c r="E14">
-        <v>50</v>
-      </c>
-      <c r="F14">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>15</v>
-      </c>
-      <c r="H14">
-        <v>85</v>
-      </c>
-      <c r="I14">
-        <v>85</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
       <c r="L14">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="O14">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>6</v>
+      </c>
+      <c r="AD14">
+        <v>6</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>6</v>
+      </c>
+      <c r="AG14">
+        <v>6</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>4</v>
+      </c>
+      <c r="AJ14">
+        <v>6</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>4</v>
+      </c>
+      <c r="AM14">
         <v>5</v>
       </c>
-      <c r="R14">
-        <v>5</v>
-      </c>
-      <c r="S14">
-        <v>2</v>
-      </c>
-      <c r="T14">
-        <v>27</v>
-      </c>
-      <c r="U14">
-        <v>27</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>3</v>
-      </c>
-      <c r="X14">
-        <v>3</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>4</v>
-      </c>
-      <c r="AA14">
-        <v>4</v>
-      </c>
-      <c r="AB14">
-        <v>6</v>
-      </c>
-      <c r="AC14">
-        <v>25</v>
-      </c>
-      <c r="AD14">
-        <v>25</v>
-      </c>
-      <c r="AE14">
-        <v>6</v>
-      </c>
-      <c r="AF14">
-        <v>25</v>
-      </c>
-      <c r="AG14">
-        <v>25</v>
-      </c>
-      <c r="AH14">
-        <v>4</v>
-      </c>
-      <c r="AI14">
-        <v>12</v>
-      </c>
-      <c r="AJ14">
-        <v>12</v>
-      </c>
-      <c r="AK14">
-        <v>5</v>
-      </c>
-      <c r="AL14">
-        <v>22</v>
-      </c>
-      <c r="AM14">
-        <v>22</v>
-      </c>
       <c r="AN14">
         <v>0</v>
       </c>
       <c r="AO14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AP14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AS14">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -2654,91 +2654,91 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F15">
+        <v>25</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>54</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>17</v>
+      </c>
+      <c r="O15">
+        <v>35</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
         <v>3</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>40</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>2</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>2</v>
-      </c>
-      <c r="O15">
-        <v>24</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>1</v>
-      </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AH15">
         <v>0</v>
@@ -2747,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="AJ15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK15">
         <v>0</v>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="AM15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN15">
         <v>0</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="16" spans="1:45">
       <c r="A16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>59</v>
@@ -2794,16 +2794,16 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="U16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2866,16 +2866,16 @@
         <v>0</v>
       </c>
       <c r="AD16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE16">
         <v>0</v>
       </c>
       <c r="AF16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG16">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AH16">
         <v>0</v>
@@ -2884,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="AJ16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK16">
         <v>0</v>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="AM16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AN16">
         <v>0</v>
@@ -2916,7 +2916,7 @@
     </row>
     <row r="17" spans="1:45">
       <c r="A17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>60</v>
@@ -2925,22 +2925,22 @@
         <v>84</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I17">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -2949,88 +2949,88 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O17">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>8</v>
+      </c>
+      <c r="U17">
+        <v>8</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>2</v>
+      </c>
+      <c r="AA17">
+        <v>2</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
         <v>5</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
+      <c r="AG17">
         <v>5</v>
       </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>0</v>
-      </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
-      <c r="AC17">
-        <v>0</v>
-      </c>
-      <c r="AD17">
-        <v>1</v>
-      </c>
-      <c r="AE17">
-        <v>0</v>
-      </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-      <c r="AG17">
-        <v>15</v>
-      </c>
       <c r="AH17">
         <v>0</v>
       </c>
       <c r="AI17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK17">
         <v>0</v>
       </c>
       <c r="AL17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AN17">
         <v>0</v>
@@ -3045,10 +3045,10 @@
         <v>0</v>
       </c>
       <c r="AR17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:45">
@@ -3065,19 +3065,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="I18">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -3086,17 +3086,17 @@
         <v>3</v>
       </c>
       <c r="L18">
+        <v>7</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <v>3</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>7</v>
       </c>
-      <c r="N18">
-        <v>47</v>
-      </c>
-      <c r="O18">
-        <v>49</v>
-      </c>
       <c r="P18">
         <v>0</v>
       </c>
@@ -3107,67 +3107,67 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <v>0</v>
       </c>
       <c r="W18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18">
         <v>0</v>
       </c>
       <c r="Z18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB18">
         <v>0</v>
       </c>
       <c r="AC18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AD18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF18">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="AG18">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="AH18">
         <v>0</v>
       </c>
       <c r="AI18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK18">
         <v>0</v>
       </c>
       <c r="AL18">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AM18">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AN18">
         <v>0</v>
@@ -3199,40 +3199,40 @@
         <v>86</v>
       </c>
       <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>49</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
         <v>7</v>
       </c>
-      <c r="E19">
-        <v>15</v>
-      </c>
-      <c r="F19">
-        <v>20</v>
-      </c>
-      <c r="G19">
-        <v>7</v>
-      </c>
-      <c r="H19">
-        <v>20</v>
-      </c>
-      <c r="I19">
-        <v>48</v>
-      </c>
-      <c r="J19">
-        <v>7</v>
-      </c>
-      <c r="K19">
-        <v>14</v>
-      </c>
       <c r="L19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N19">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="O19">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="20" spans="1:45">
       <c r="A20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>63</v>
@@ -3336,112 +3336,112 @@
         <v>87</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P20">
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20">
         <v>0</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20">
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB20">
         <v>0</v>
       </c>
       <c r="AC20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE20">
         <v>0</v>
       </c>
       <c r="AF20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG20">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AH20">
         <v>0</v>
       </c>
       <c r="AI20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK20">
         <v>0</v>
       </c>
       <c r="AL20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN20">
         <v>0</v>
@@ -3476,37 +3476,37 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F21">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I21">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L21">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O21">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
         <v>0</v>
@@ -3524,7 +3524,7 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -3533,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="X21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y21">
         <v>0</v>
@@ -3542,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="AA21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB21">
         <v>0</v>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="AD21">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="AE21">
         <v>0</v>
@@ -3560,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="AG21">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="AH21">
         <v>0</v>
@@ -3569,16 +3569,16 @@
         <v>0</v>
       </c>
       <c r="AJ21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK21">
         <v>0</v>
       </c>
       <c r="AL21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AN21">
         <v>0</v>
@@ -3587,7 +3587,7 @@
         <v>0</v>
       </c>
       <c r="AP21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ21">
         <v>0</v>
@@ -3596,12 +3596,12 @@
         <v>0</v>
       </c>
       <c r="AS21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:45">
       <c r="A22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
@@ -3610,58 +3610,58 @@
         <v>89</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P22">
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S22">
         <v>0</v>
       </c>
       <c r="T22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -3682,40 +3682,40 @@
         <v>0</v>
       </c>
       <c r="AB22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AD22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AE22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AG22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH22">
         <v>0</v>
       </c>
       <c r="AI22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AK22">
         <v>0</v>
       </c>
       <c r="AL22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AM22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AN22">
         <v>0</v>
@@ -3747,130 +3747,130 @@
         <v>90</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>13</v>
+      </c>
+      <c r="F23">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>120</v>
+      </c>
+      <c r="I23">
+        <v>129</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
         <v>3</v>
       </c>
-      <c r="E23">
-        <v>15</v>
-      </c>
-      <c r="F23">
-        <v>15</v>
-      </c>
-      <c r="G23">
+      <c r="L23">
         <v>3</v>
       </c>
-      <c r="H23">
-        <v>27</v>
-      </c>
-      <c r="I23">
-        <v>27</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
       <c r="M23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N23">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="O23">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>4</v>
+      </c>
+      <c r="U23">
+        <v>4</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>2</v>
+      </c>
+      <c r="AA23">
+        <v>2</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
         <v>8</v>
       </c>
-      <c r="R23">
+      <c r="AD23">
         <v>8</v>
       </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="T23">
-        <v>8</v>
-      </c>
-      <c r="U23">
-        <v>8</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-      <c r="Z23">
-        <v>1</v>
-      </c>
-      <c r="AA23">
-        <v>1</v>
-      </c>
-      <c r="AB23">
-        <v>0</v>
-      </c>
-      <c r="AC23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>0</v>
-      </c>
       <c r="AE23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF23">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="AG23">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="AH23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AJ23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AK23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL23">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="AM23">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="AN23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:45">
@@ -3884,112 +3884,112 @@
         <v>91</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="W24">
+        <v>2</v>
+      </c>
+      <c r="X24">
+        <v>2</v>
+      </c>
+      <c r="Y24">
+        <v>2</v>
+      </c>
+      <c r="Z24">
+        <v>3</v>
+      </c>
+      <c r="AA24">
+        <v>4</v>
+      </c>
+      <c r="AB24">
         <v>5</v>
       </c>
-      <c r="F24">
-        <v>7</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
+      <c r="AC24">
         <v>5</v>
       </c>
-      <c r="I24">
-        <v>7</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
+      <c r="AD24">
         <v>5</v>
       </c>
-      <c r="L24">
-        <v>7</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
+      <c r="AE24">
         <v>5</v>
       </c>
-      <c r="O24">
-        <v>7</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-      <c r="Y24">
-        <v>0</v>
-      </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-      <c r="AA24">
-        <v>0</v>
-      </c>
-      <c r="AB24">
-        <v>0</v>
-      </c>
-      <c r="AC24">
-        <v>0</v>
-      </c>
-      <c r="AD24">
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
       <c r="AF24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN24">
         <v>0</v>
@@ -4021,58 +4021,58 @@
         <v>92</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F25">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="H25">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I25">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M25">
         <v>1</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="U25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V25">
         <v>0</v>
@@ -4087,46 +4087,46 @@
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC25">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD25">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF25">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AG25">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AH25">
         <v>0</v>
       </c>
       <c r="AI25">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AJ25">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AK25">
         <v>0</v>
       </c>
       <c r="AL25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AM25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AN25">
         <v>0</v>
@@ -4141,10 +4141,10 @@
         <v>0</v>
       </c>
       <c r="AR25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>